<commit_message>
set up for python3
</commit_message>
<xml_diff>
--- a/RemoteYearBot/SampleData_RealAnon2020/forBot_StudentRequestList.xlsx
+++ b/RemoteYearBot/SampleData_RealAnon2020/forBot_StudentRequestList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/github/interviewScheduler/SampleData_RealAnon2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/github/interviewScheduler/RemoteYearBot/SampleData_RealAnon2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DC491B-6A4D-514F-8AE2-F64B294720E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5A18C6-065F-884F-9938-35A4E99B2AFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3520" yWindow="1980" windowWidth="20600" windowHeight="24040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
   <si>
     <t>Asterisk</t>
   </si>
@@ -190,13 +190,28 @@
   </si>
   <si>
     <t>Ogawa, Alyssa</t>
+  </si>
+  <si>
+    <t>Timezone</t>
+  </si>
+  <si>
+    <t>PST</t>
+  </si>
+  <si>
+    <t>EST</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -208,6 +223,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -248,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -257,6 +280,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,395 +600,477 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="95.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="5" max="5" width="95.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B4">
-        <v>0</v>
+      <c r="B4" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B5">
-        <v>0</v>
+      <c r="B5" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B6">
-        <v>0</v>
+      <c r="B6" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="3">
-        <v>0</v>
+      <c r="B7" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C7" s="3">
         <v>0</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B8">
-        <v>0</v>
+      <c r="B8" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B9">
-        <v>1</v>
+      <c r="B9" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B10">
-        <v>0</v>
+      <c r="B10" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B11">
-        <v>1</v>
+      <c r="B11" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B12">
-        <v>0</v>
+      <c r="B12" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B13">
-        <v>1</v>
+      <c r="B13" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B14">
-        <v>0</v>
+      <c r="B14" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B15">
-        <v>0</v>
+      <c r="B15" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B16">
-        <v>0</v>
+      <c r="B16" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B17">
-        <v>0</v>
+      <c r="B17" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B18">
-        <v>0</v>
+      <c r="B18" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B19">
-        <v>0</v>
+      <c r="B19" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B20">
-        <v>0</v>
+      <c r="B20" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B21">
-        <v>0</v>
+      <c r="B21" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B22">
-        <v>0</v>
+      <c r="B22" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B23">
-        <v>0</v>
+      <c r="B23" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B24">
-        <v>0</v>
+      <c r="B24" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B25">
-        <v>0</v>
+      <c r="B25" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B26">
-        <v>1</v>
+      <c r="B26" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B27">
-        <v>0</v>
+      <c r="B27" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G28">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H28">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Python3 translation except post-Metro part
</commit_message>
<xml_diff>
--- a/RemoteYearBot/SampleData_RealAnon2020/forBot_StudentRequestList.xlsx
+++ b/RemoteYearBot/SampleData_RealAnon2020/forBot_StudentRequestList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/github/interviewScheduler/RemoteYearBot/SampleData_RealAnon2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5A18C6-065F-884F-9938-35A4E99B2AFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D55A3BF-299F-2646-8E95-F7CA09B06929}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="1980" windowWidth="20600" windowHeight="24040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50320" yWindow="460" windowWidth="17460" windowHeight="25720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -603,7 +603,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add option for partial student
</commit_message>
<xml_diff>
--- a/RemoteYearBot/SampleData_RealAnon2020/forBot_StudentRequestList.xlsx
+++ b/RemoteYearBot/SampleData_RealAnon2020/forBot_StudentRequestList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/github/interviewScheduler/RemoteYearBot/SampleData_RealAnon2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D55A3BF-299F-2646-8E95-F7CA09B06929}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6A8975-A3C1-3F43-8891-682FCA906C38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50320" yWindow="460" windowWidth="17460" windowHeight="25720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8680" yWindow="460" windowWidth="17460" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
   <si>
     <t>Asterisk</t>
   </si>
@@ -205,13 +205,22 @@
   </si>
   <si>
     <t>India</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
+    <t>Thu</t>
+  </si>
+  <si>
+    <t>Fri</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -231,6 +240,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -271,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -286,6 +303,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,37 +618,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="5" max="5" width="95.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.83203125" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="95.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>49</v>
       </c>
@@ -643,11 +675,20 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -660,11 +701,20 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
@@ -677,11 +727,20 @@
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
@@ -694,11 +753,20 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -711,11 +779,20 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -728,11 +805,20 @@
       <c r="D7" s="3">
         <v>0</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -745,11 +831,20 @@
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
@@ -762,11 +857,20 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
@@ -779,11 +883,20 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
@@ -796,11 +909,20 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
@@ -813,11 +935,20 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -830,11 +961,20 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
@@ -847,11 +987,20 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
@@ -864,11 +1013,20 @@
       <c r="D15">
         <v>0</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -881,11 +1039,20 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
@@ -898,11 +1065,20 @@
       <c r="D17">
         <v>0</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
@@ -915,11 +1091,20 @@
       <c r="D18">
         <v>0</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
@@ -932,11 +1117,20 @@
       <c r="D19">
         <v>0</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
@@ -949,11 +1143,20 @@
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>48</v>
       </c>
@@ -966,11 +1169,20 @@
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -983,11 +1195,20 @@
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -1000,11 +1221,20 @@
       <c r="D23">
         <v>0</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>54</v>
       </c>
@@ -1017,11 +1247,20 @@
       <c r="D24">
         <v>1</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>42</v>
       </c>
@@ -1034,8 +1273,17 @@
       <c r="D25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>52</v>
       </c>
@@ -1048,11 +1296,20 @@
       <c r="D26">
         <v>1</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>53</v>
       </c>
@@ -1065,12 +1322,21 @@
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H28">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K28">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>